<commit_message>
CHANGES  WITH UNIT TEST
</commit_message>
<xml_diff>
--- a/instance/reports/unit_test_report.xlsx
+++ b/instance/reports/unit_test_report.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,7 +446,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>test_login_page_loads (tests.login_test.LoginTestCase.test_login_page_loads)</t>
+          <t>test_create_appointment (appointment_test.AppointmentTestCase.test_create_appointment)</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -461,14 +461,14 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2025-11-24 11:35:30</t>
+          <t>2025-11-26 20:23:22</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>test_logout (tests.login_test.LoginTestCase.test_logout)</t>
+          <t>test_invalid_date_time (appointment_test.AppointmentTestCase.test_invalid_date_time)</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -483,14 +483,14 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2025-11-24 11:35:30</t>
+          <t>2025-11-26 20:23:22</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>test_missing_password_fails (tests.login_test.LoginTestCase.test_missing_password_fails)</t>
+          <t>test_missing_required_fields (appointment_test.AppointmentTestCase.test_missing_required_fields)</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -505,14 +505,14 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2025-11-24 11:35:30</t>
+          <t>2025-11-26 20:23:22</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>test_missing_username_fails (tests.login_test.LoginTestCase.test_missing_username_fails)</t>
+          <t>test_upcoming_appointments_visible (appointment_test.AppointmentTestCase.test_upcoming_appointments_visible)</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -527,14 +527,14 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2025-11-24 11:35:30</t>
+          <t>2025-11-26 20:23:22</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>test_successful_login (tests.login_test.LoginTestCase.test_successful_login)</t>
+          <t>test_reply_blocked (forum_test.ForumTestCase.test_reply_blocked)</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -549,14 +549,14 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2025-11-24 11:35:30</t>
+          <t>2025-11-26 20:23:22</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>test_wrong_password_fails (tests.login_test.LoginTestCase.test_wrong_password_fails)</t>
+          <t>test_reply_creation (forum_test.ForumTestCase.test_reply_creation)</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -571,7 +571,249 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2025-11-24 11:35:30</t>
+          <t>2025-11-26 20:23:22</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>test_safe_post_persists (forum_test.ForumTestCase.test_safe_post_persists)</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Test passed</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2025-11-26 20:23:22</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>test_unsafe_post_blocked (forum_test.ForumTestCase.test_unsafe_post_blocked)</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Test passed</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>2025-11-26 20:23:22</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>test_login_page_loads (login_test.LoginTestCase.test_login_page_loads)</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Test passed</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>2025-11-26 20:23:22</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>test_logout (login_test.LoginTestCase.test_logout)</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Test passed</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>2025-11-26 20:23:22</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>test_missing_password_fails (login_test.LoginTestCase.test_missing_password_fails)</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Test passed</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>2025-11-26 20:23:22</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>test_missing_username_fails (login_test.LoginTestCase.test_missing_username_fails)</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Test passed</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>2025-11-26 20:23:22</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>test_successful_login (login_test.LoginTestCase.test_successful_login)</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Test passed</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>2025-11-26 20:23:22</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>test_wrong_password_fails (login_test.LoginTestCase.test_wrong_password_fails)</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Test passed</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>2025-11-26 20:23:22</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>test_missing_required_fields (profile_test.ProfileTestCase.test_missing_required_fields)</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Test passed</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>2025-11-26 20:23:22</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>test_profile_creation (profile_test.ProfileTestCase.test_profile_creation)</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Test passed</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>2025-11-26 20:23:22</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>test_profile_update (profile_test.ProfileTestCase.test_profile_update)</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Test passed</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>2025-11-26 20:23:22</t>
         </is>
       </c>
     </row>

</xml_diff>